<commit_message>
added WorkID; updated insert data
</commit_message>
<xml_diff>
--- a/ProjectData.xlsx
+++ b/ProjectData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yenny\Desktop\Langara\T3 - 2022 Summer\CPSC-2221-001-Database System\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yenny\Desktop\Langara\T3 - 2022 Summer\CPSC-2221-001-Database System\Project\Students-Clubs-Management-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7FC2B5-ABCD-4521-B2CF-5D7A546BB333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6C7F7E-BB8B-4302-9783-D34281FF9E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" tabRatio="686" activeTab="3" xr2:uid="{4E4250F2-02E0-442C-A677-9B48E0158598}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="144">
   <si>
     <t>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Hou</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Hector</t>
   </si>
   <si>
@@ -416,9 +413,6 @@
     <t>INSERT INTO Member_WorksOn_Project (MemberID, ProjectCode, MemberPortion) VALUES (</t>
   </si>
   <si>
-    <t>INSERT INTO Alumnus_WorkHistory (AlumnusID, Company, Position, StartDate, EndDate) VALUES (</t>
-  </si>
-  <si>
     <t>Yahoo</t>
   </si>
   <si>
@@ -462,6 +456,24 @@
   </si>
   <si>
     <t>2022/09/20</t>
+  </si>
+  <si>
+    <t>WorkID</t>
+  </si>
+  <si>
+    <t>2019/08/01</t>
+  </si>
+  <si>
+    <t>2020/07/31</t>
+  </si>
+  <si>
+    <t>INSERT INTO Alumnus_WorkHistory (AlumnusID, WorkID, Company, Position, StartDate, EndDate) VALUES (</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>AL</t>
   </si>
 </sst>
 </file>
@@ -861,7 +873,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -886,17 +898,17 @@
         <v>10001001</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F4" t="str">
         <f>_xlfn.CONCAT($A$1,A4,",'",B4,"','",C4,"','",D4,"'",$B$1)</f>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001001,'Hector','Onato','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001001,'Hector','Onato','ST');</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -910,11 +922,11 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F22" si="0">_xlfn.CONCAT($A$1,A5,",'",B5,"','",C5,"','",D5,"'",$B$1)</f>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001002,'Yan Fung Yenny','Hou','S');</v>
+        <f t="shared" ref="F5:F7" si="0">_xlfn.CONCAT($A$1,A5,",'",B5,"','",C5,"','",D5,"'",$B$1)</f>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001002,'Yan Fung Yenny','Hou','ST');</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -922,17 +934,17 @@
         <v>10001003</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001003,'Blanche','Sitznski','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001003,'Blanche','Sitznski','ST');</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -940,17 +952,17 @@
         <v>10001004</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001004,'Natasha','Romanoff','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001004,'Natasha','Romanoff','ST');</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -958,17 +970,17 @@
         <v>10001005</v>
       </c>
       <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="F8" t="str">
         <f>_xlfn.CONCAT($A$1,A8,",'",B8,"','",C8,"','",D8,"'",$B$1)</f>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001005,'Landi','Umberto','A');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001005,'Landi','Umberto','AL');</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -976,17 +988,17 @@
         <v>10001006</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" ref="F9:F23" si="1">_xlfn.CONCAT($A$1,A9,",'",B9,"','",C9,"','",D9,"'",$B$1)</f>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001006,'Fred','Myers','A');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001006,'Fred','Myers','AL');</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -994,17 +1006,17 @@
         <v>10001007</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001007,'Marc','Scott','A');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001007,'Marc','Scott','AL');</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1012,17 +1024,17 @@
         <v>10001008</v>
       </c>
       <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001008,'Hugo','Etherlinck','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001008,'Hugo','Etherlinck','ST');</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1030,17 +1042,17 @@
         <v>10001009</v>
       </c>
       <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001009,'Mora','Cathrine ','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001009,'Mora','Cathrine ','ST');</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1048,17 +1060,17 @@
         <v>10001010</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001010,'Scott ','Summers','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001010,'Scott ','Summers','ST');</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1066,17 +1078,17 @@
         <v>10001011</v>
       </c>
       <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
         <v>70</v>
       </c>
-      <c r="C14" t="s">
-        <v>71</v>
-      </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001011,'Yuriko','Oyama','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001011,'Yuriko','Oyama','ST');</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1084,17 +1096,17 @@
         <v>10001012</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001012,'Wilson','Wade','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001012,'Wilson','Wade','ST');</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1102,17 +1114,17 @@
         <v>10001013</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001013,'Bram ','Velsing','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001013,'Bram ','Velsing','ST');</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1120,17 +1132,17 @@
         <v>10001014</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001014,'Daisy ','Johnson','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001014,'Daisy ','Johnson','ST');</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1138,17 +1150,17 @@
         <v>10001015</v>
       </c>
       <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
         <v>78</v>
       </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001015,'Elektra','Natchios','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001015,'Elektra','Natchios','ST');</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1156,17 +1168,17 @@
         <v>10001016</v>
       </c>
       <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001016,'Max','Dillon','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001016,'Max','Dillon','ST');</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1174,17 +1186,17 @@
         <v>10001017</v>
       </c>
       <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" t="s">
-        <v>83</v>
-      </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001017,'Ivory ','Shadow','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001017,'Ivory ','Shadow','ST');</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1192,17 +1204,17 @@
         <v>10001018</v>
       </c>
       <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
         <v>84</v>
       </c>
-      <c r="C21" t="s">
-        <v>85</v>
-      </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001018,'Dan','Rubenstein','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001018,'Dan','Rubenstein','ST');</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1210,17 +1222,17 @@
         <v>10001019</v>
       </c>
       <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
-        <v>87</v>
-      </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001019,'Norman','Osborn','S');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001019,'Norman','Osborn','ST');</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1228,17 +1240,17 @@
         <v>10001020</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001020,'Jack','Danner','A');</v>
+        <v>INSERT INTO Member (MemberID, FirstName, LastName, MemberType) VALUES (10001020,'Jack','Danner','AL');</v>
       </c>
     </row>
   </sheetData>
@@ -1266,7 +1278,7 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1291,7 +1303,7 @@
         <v>10001001</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="str">
         <f>_xlfn.CONCAT($A$1,A4,",",B4,",'",C4,"'",$B$1)</f>
@@ -1306,7 +1318,7 @@
         <v>10001001</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ref="E5:E7" si="0">_xlfn.CONCAT($A$1,A5,",",B5,",'",C5,"'",$B$1)</f>
@@ -1321,7 +1333,7 @@
         <v>10001002</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1336,7 +1348,7 @@
         <v>10001003</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1360,10 +1372,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1374,10 +1386,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1394,7 +1406,7 @@
         <v>10001004</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="str">
         <f>_xlfn.CONCAT($A$1,A4,",",B4,,",",C4,",'",D4,"'",$B$1)</f>
@@ -1412,7 +1424,7 @@
         <v>10001005</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="str">
         <f>_xlfn.CONCAT($A$1,A5,",",B5,,",",C5,",'",D5,"'",$B$1)</f>
@@ -1430,7 +1442,7 @@
         <v>10001006</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ref="F6:F14" si="0">_xlfn.CONCAT($A$1,A6,",",B6,,",",C6,",'",D6,"'",$B$1)</f>
@@ -1448,7 +1460,7 @@
         <v>10001008</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -1466,7 +1478,7 @@
         <v>10001008</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -1484,7 +1496,7 @@
         <v>10001009</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -1502,7 +1514,7 @@
         <v>10001010</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -1520,7 +1532,7 @@
         <v>10001011</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -1538,7 +1550,7 @@
         <v>10001012</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -1556,7 +1568,7 @@
         <v>10001013</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -1574,7 +1586,7 @@
         <v>10001014</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -1591,7 +1603,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
@@ -1608,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1657,29 +1669,29 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="G4">
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4" t="str">
-        <f>_xlfn.CONCAT($A$1,A4,",",B4,",",C4,",'",D5,"','",E4,"','",F4,"',",G4,",'",H4,"',",I4,",'",J4,"'",$B$1)</f>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (101,1000,1,'How to write your first Java program','2022/06/15','12:30:00',5,'A',1,'122A');</v>
+        <f>_xlfn.CONCAT($A$1,A4,",",B4,",",C4,",'",D4,"','",E4,"','",F4,"',",G4,",'",H4,"',",I4,",'",J4,"'",$B$1)</f>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (101,1000,1,'Become a Data Analyst','2022/06/15','12:30:00',5,'A',1,'122A');</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1693,29 +1705,29 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5">
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" ref="L5:L10" si="0">_xlfn.CONCAT($A$1,A5,",",B5,",",C5,",'",D6,"','",E5,"','",F5,"',",G5,",'",H5,"',",I5,",'",J5,"'",$B$1)</f>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (102,1000,2,'Java Summer Code Camp','2022/07/04','09:30:00',5,'B',0,'019');</v>
+        <f t="shared" ref="L5:L10" si="0">_xlfn.CONCAT($A$1,A5,",",B5,",",C5,",'",D5,"','",E5,"','",F5,"',",G5,",'",H5,"',",I5,",'",J5,"'",$B$1)</f>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (102,1000,2,'How to write your first Java program','2022/07/04','09:30:00',5,'B',0,'019');</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1729,29 +1741,29 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="G6">
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (103,1000,2,'Biology Club Orientation - Plant Research','2022/08/06','09:30:00',20,'A',1,'122A');</v>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (103,1000,2,'Java Summer Code Camp','2022/08/06','09:30:00',20,'A',1,'122A');</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1765,29 +1777,29 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (201,2000,1,'Biology Club Orientation - Insect Research','2022/08/16','10:00:00',0,'T',5,'530');</v>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (201,2000,1,'Biology Club Orientation - Plant Research','2022/08/16','10:00:00',0,'T',5,'530');</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1801,29 +1813,29 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I8">
         <v>5</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (202,2000,2,'Biology Club Orientation - Animal Research','2022/08/16','10:00:00',0,'T',5,'530');</v>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (202,2000,2,'Biology Club Orientation - Insect Research','2022/08/16','10:00:00',0,'T',5,'530');</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1837,29 +1849,29 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9">
         <v>5</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (203,2000,3,'Latin Competition','2022/08/16','10:00:00',0,'T',5,'530');</v>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (203,2000,3,'Biology Club Orientation - Animal Research','2022/08/16','10:00:00',0,'T',5,'530');</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1873,29 +1885,29 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (401,4000,1,'','2022/09/20','08:30:00',10,'G',1,'105');</v>
+        <v>INSERT INTO Event (EventID, ClubID, GroupID, EventSubject, EventDate, EventTime, RegistrationFee, Building, BuildingFloor, Room) VALUES (401,4000,1,'Latin Competition','2022/09/20','08:30:00',10,'G',1,'105');</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1956,15 +1968,15 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1973,10 +1985,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>19</v>
@@ -1984,7 +1996,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -1993,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4">
         <v>6000</v>
@@ -2005,7 +2017,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -2014,7 +2026,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5">
         <v>6000</v>
@@ -2026,7 +2038,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>2000</v>
@@ -2035,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6">
         <v>5000</v>
@@ -2047,7 +2059,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>2000</v>
@@ -2056,7 +2068,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -2068,7 +2080,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8">
         <v>2000</v>
@@ -2077,7 +2089,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -2089,7 +2101,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9">
         <v>3000</v>
@@ -2098,7 +2110,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9">
         <v>4000</v>
@@ -2125,10 +2137,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2156,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="str">
-        <f>_xlfn.CONCAT($A$1,A4,",",B4,",",C4,$B$1)</f>
+        <f t="shared" ref="E4:E25" si="0">_xlfn.CONCAT($A$1,A4,",",B4,",",C4,$B$1)</f>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001001,1000,2);</v>
       </c>
     </row>
@@ -2171,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <f>_xlfn.CONCAT($A$1,A5,",",B5,",",C5,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001001,2000,1);</v>
       </c>
     </row>
@@ -2186,7 +2198,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="str">
-        <f>_xlfn.CONCAT($A$1,A6,",",B6,",",C6,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001002,3000,2);</v>
       </c>
     </row>
@@ -2201,7 +2213,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <f>_xlfn.CONCAT($A$1,A7,",",B7,",",C7,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001003,4000,1);</v>
       </c>
     </row>
@@ -2216,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <f>_xlfn.CONCAT($A$1,A8,",",B8,",",C8,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001004,1000,1);</v>
       </c>
     </row>
@@ -2231,7 +2243,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="str">
-        <f>_xlfn.CONCAT($A$1,A9,",",B9,",",C9,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001005,1000,2);</v>
       </c>
     </row>
@@ -2246,7 +2258,7 @@
         <v>3</v>
       </c>
       <c r="E10" t="str">
-        <f>_xlfn.CONCAT($A$1,A10,",",B10,",",C10,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001006,1000,3);</v>
       </c>
     </row>
@@ -2261,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <f>_xlfn.CONCAT($A$1,A11,",",B11,",",C11,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001007,1000,1);</v>
       </c>
     </row>
@@ -2276,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <f>_xlfn.CONCAT($A$1,A12,",",B12,",",C12,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001008,2000,1);</v>
       </c>
     </row>
@@ -2291,7 +2303,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="str">
-        <f>_xlfn.CONCAT($A$1,A13,",",B13,",",C13,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001008,2000,2);</v>
       </c>
     </row>
@@ -2306,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="str">
-        <f>_xlfn.CONCAT($A$1,A14,",",B14,",",C14,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001009,2000,3);</v>
       </c>
     </row>
@@ -2321,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f>_xlfn.CONCAT($A$1,A15,",",B15,",",C15,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001010,3000,1);</v>
       </c>
     </row>
@@ -2336,7 +2348,7 @@
         <v>2</v>
       </c>
       <c r="E16" t="str">
-        <f>_xlfn.CONCAT($A$1,A16,",",B16,",",C16,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001011,3000,2);</v>
       </c>
     </row>
@@ -2351,7 +2363,7 @@
         <v>3</v>
       </c>
       <c r="E17" t="str">
-        <f>_xlfn.CONCAT($A$1,A17,",",B17,",",C17,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001012,3000,3);</v>
       </c>
     </row>
@@ -2366,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="str">
-        <f>_xlfn.CONCAT($A$1,A18,",",B18,",",C18,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001013,4000,1);</v>
       </c>
     </row>
@@ -2381,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <f>_xlfn.CONCAT($A$1,A19,",",B19,",",C19,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001014,4000,2);</v>
       </c>
     </row>
@@ -2396,7 +2408,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <f>_xlfn.CONCAT($A$1,A20,",",B20,",",C20,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001015,3000,2);</v>
       </c>
     </row>
@@ -2411,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="E21" t="str">
-        <f>_xlfn.CONCAT($A$1,A21,",",B21,",",C21,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001016,2000,2);</v>
       </c>
     </row>
@@ -2426,7 +2438,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="str">
-        <f>_xlfn.CONCAT($A$1,A22,",",B22,",",C22,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001017,3000,1);</v>
       </c>
     </row>
@@ -2441,7 +2453,7 @@
         <v>3</v>
       </c>
       <c r="E23" t="str">
-        <f>_xlfn.CONCAT($A$1,A23,",",B23,",",C23,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001018,3000,3);</v>
       </c>
     </row>
@@ -2456,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <f>_xlfn.CONCAT($A$1,A24,",",B24,",",C24,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001019,4000,2);</v>
       </c>
     </row>
@@ -2471,7 +2483,7 @@
         <v>3</v>
       </c>
       <c r="E25" t="str">
-        <f>_xlfn.CONCAT($A$1,A25,",",B25,",",C25,$B$1)</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO Member_Joins_Group (MemberID, ClubID, GroupID) VALUES (10001020,2000,3);</v>
       </c>
     </row>
@@ -2498,10 +2510,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2509,10 +2521,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
@@ -2523,7 +2535,7 @@
         <v>10001001</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4">
         <v>1500</v>
@@ -2538,7 +2550,7 @@
         <v>10001003</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5">
         <v>1500</v>
@@ -2553,7 +2565,7 @@
         <v>10001003</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6">
         <v>1000</v>
@@ -2568,7 +2580,7 @@
         <v>10001004</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7">
         <v>2000</v>
@@ -2583,7 +2595,7 @@
         <v>10001005</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8">
         <v>1500</v>
@@ -2598,7 +2610,7 @@
         <v>10001008</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>500</v>
@@ -2613,7 +2625,7 @@
         <v>10001008</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10">
         <v>600</v>
@@ -2628,7 +2640,7 @@
         <v>10001001</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>700</v>
@@ -2643,7 +2655,7 @@
         <v>10001009</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12">
         <v>700</v>
@@ -2658,7 +2670,7 @@
         <v>10001020</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13">
         <v>700</v>
@@ -2673,7 +2685,7 @@
         <v>10001002</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14">
         <v>500</v>
@@ -2688,7 +2700,7 @@
         <v>10001015</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15">
         <v>500</v>
@@ -2703,7 +2715,7 @@
         <v>10001011</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16">
         <v>500</v>
@@ -2720,128 +2732,167 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB47892D-350D-4478-A27E-B1034A2029BF}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H4" sqref="H4:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>10001006</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>129</v>
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" t="str">
-        <f>_xlfn.CONCAT($A$1,A4,",'",B4,"','",C4,"','",D4,"','",E4,"'",$B$1)</f>
-        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, Company, Position, StartDate, EndDate) VALUES (10001006,'Google','Software Engineer','2018/10/01','2021/09/30');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>127</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT($A$1,A4,",",B4,",'",C4,"','",D4,"','",E4,"','",F4,"'",$C$1)</f>
+        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, WorkID, Company, Position, StartDate, EndDate) VALUES (10001006,1,'Google','Software Engineer','2018/10/01','2021/09/30');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>10001006</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
+      <c r="B5">
+        <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="7" t="str">
-        <f>_xlfn.CONCAT($A$1,A5,",'",B5,"','",C5,"','",D5,"',",E5,$B$1)</f>
-        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, Company, Position, StartDate, EndDate) VALUES (10001006,'Facebook','Full Stack Web Developer','2021/11/01',NULL);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="7" t="str">
+        <f>_xlfn.CONCAT($A$1,A5,",",B5,",'",C5,"','",D5,"','",E5,"',",F5,$C$1)</f>
+        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, WorkID, Company, Position, StartDate, EndDate) VALUES (10001006,2,'Facebook','Full Stack Web Developer','2021/11/01',NULL);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>10001007</v>
       </c>
-      <c r="B6" t="s">
-        <v>125</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="7" t="str">
-        <f>_xlfn.CONCAT($A$1,A6,",'",B6,"','",C6,"','",D6,"',",E6,$B$1)</f>
-        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, Company, Position, StartDate, EndDate) VALUES (10001007,'Yahoo','Data Analyst','2020/09/01',NULL);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="7" t="str">
+        <f>_xlfn.CONCAT($A$1,A6,",",B6,",'",C6,"','",D6,"','",E6,"',",F6,$C$1)</f>
+        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, WorkID, Company, Position, StartDate, EndDate) VALUES (10001007,1,'Yahoo','Data Analyst','2020/09/01',NULL);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>10001005</v>
       </c>
-      <c r="B7" t="s">
-        <v>127</v>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="7" t="str">
-        <f>_xlfn.CONCAT($A$1,A7,",'",B7,"','",C7,"','",D7,"',",E7,$B$1)</f>
-        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, Company, Position, StartDate, EndDate) VALUES (10001005,'Amazon','System Analyst','2021/04/01',NULL);</v>
+        <v>125</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT($A$1,A7,",",B7,",'",C7,"','",D7,"','",E7,"','",F7,"'",$C$1)</f>
+        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, WorkID, Company, Position, StartDate, EndDate) VALUES (10001005,1,'Amazon','Software Engineer','2019/08/01','2020/07/31');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>10001005</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="7" t="str">
+        <f>_xlfn.CONCAT($A$1,A8,",",B8,",'",C8,"','",D8,"','",E8,"',",F8,$C$1)</f>
+        <v>INSERT INTO Alumnus_WorkHistory (AlumnusID, WorkID, Company, Position, StartDate, EndDate) VALUES (10001005,2,'Amazon','System Analyst','2021/04/01',NULL);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>